<commit_message>
Update da aula 04 / Finalizada aula 05
</commit_message>
<xml_diff>
--- a/edge_computing_computer_systems_2023.xlsx
+++ b/edge_computing_computer_systems_2023.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/439d5056bbd31b7f/Documentos/Pessoal/GRADUAÇÃO/FIAP/2023/ES/ementas_contribuições/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Profissional\Empresas\FIAP\02 Aulas\Engenharia de Software\Edge Computing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{195555B1-4A74-4584-B29E-A4ACCD183809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B7215D9-1C80-434F-8B26-558FB3A6EC5D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51C01AE-DDB9-4332-8975-EF9036271EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="360" windowWidth="25440" windowHeight="15270" xr2:uid="{D49DE45F-6E56-49B0-AF9E-35E4A8BA3329}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D49DE45F-6E56-49B0-AF9E-35E4A8BA3329}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -384,6 +373,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -398,9 +390,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,23 +707,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61519789-C00C-41BB-A46E-0B2341A8977A}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="14"/>
-    </row>
-    <row r="2" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="15"/>
+    </row>
+    <row r="2" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -742,7 +731,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -750,13 +739,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
-    </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="17"/>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -764,7 +753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -772,7 +761,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>2</v>
       </c>
@@ -780,7 +769,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>3</v>
       </c>
@@ -788,7 +777,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>4</v>
       </c>
@@ -796,7 +785,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>5</v>
       </c>
@@ -804,7 +793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>6</v>
       </c>
@@ -812,7 +801,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>7</v>
       </c>
@@ -820,15 +809,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>8</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>9</v>
       </c>
@@ -836,7 +825,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>10</v>
       </c>
@@ -844,7 +833,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>11</v>
       </c>
@@ -852,23 +841,23 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>12</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>13</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>14</v>
       </c>
@@ -876,7 +865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>15</v>
       </c>
@@ -884,7 +873,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>16</v>
       </c>
@@ -892,7 +881,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>17</v>
       </c>
@@ -900,7 +889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>18</v>
       </c>
@@ -908,7 +897,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>19</v>
       </c>
@@ -916,7 +905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>20</v>
       </c>
@@ -924,13 +913,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="15" t="s">
+    <row r="26" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="17"/>
-    </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="18"/>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>1</v>
       </c>
@@ -938,7 +927,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>2</v>
       </c>
@@ -946,7 +935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>3</v>
       </c>
@@ -954,7 +943,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>4</v>
       </c>
@@ -962,7 +951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>5</v>
       </c>
@@ -970,7 +959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>6</v>
       </c>
@@ -978,7 +967,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>7</v>
       </c>
@@ -986,7 +975,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>8</v>
       </c>
@@ -994,7 +983,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>9</v>
       </c>
@@ -1002,7 +991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>10</v>
       </c>
@@ -1010,7 +999,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>11</v>
       </c>
@@ -1018,7 +1007,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>12</v>
       </c>
@@ -1026,7 +1015,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>13</v>
       </c>
@@ -1034,7 +1023,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>14</v>
       </c>
@@ -1042,7 +1031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>15</v>
       </c>
@@ -1050,7 +1039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>16</v>
       </c>
@@ -1058,7 +1047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>17</v>
       </c>
@@ -1066,7 +1055,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>18</v>
       </c>
@@ -1074,7 +1063,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>19</v>
       </c>
@@ -1082,7 +1071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Revisão das aulas do primeiro semestre e preparação das aulas do segundo
</commit_message>
<xml_diff>
--- a/edge_computing_computer_systems_2023.xlsx
+++ b/edge_computing_computer_systems_2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Profissional\Empresas\FIAP\02 Aulas\1ES\Edge Computing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Profissional\Empresas\02. FIAP\02 Aulas\1ES\Edge Computing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA125C0B-5076-42B5-BD99-791C2BECC842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EDA07F-431F-4EF7-8B74-F2931AB14B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D49DE45F-6E56-49B0-AF9E-35E4A8BA3329}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="43">
   <si>
     <t>DISCIPLINA:</t>
   </si>
@@ -248,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +277,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -394,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -453,6 +459,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,7 +777,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,6 +954,9 @@
       <c r="B13" s="13" t="s">
         <v>20</v>
       </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
@@ -1006,6 +1016,15 @@
       <c r="B17" s="13" t="s">
         <v>22</v>
       </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7">
@@ -1014,6 +1033,9 @@
       <c r="B18" s="13" t="s">
         <v>32</v>
       </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
@@ -1022,6 +1044,15 @@
       <c r="B19" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
@@ -1047,6 +1078,15 @@
       <c r="B21" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7">
@@ -1055,6 +1095,15 @@
       <c r="B22" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7">
@@ -1063,6 +1112,15 @@
       <c r="B23" s="11" t="s">
         <v>9</v>
       </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7">
@@ -1071,6 +1129,15 @@
       <c r="B24" s="11" t="s">
         <v>10</v>
       </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
@@ -1078,6 +1145,15 @@
       </c>
       <c r="B25" s="11" t="s">
         <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>